<commit_message>
clean and update with manuscript text
</commit_message>
<xml_diff>
--- a/Supplementary_Information/Table_S4.xlsx
+++ b/Supplementary_Information/Table_S4.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eanttila/Documents/GitHub/Anttila_et_al_Khuvsgul_2024/Supplementary Information/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eanttila/Documents/GitHub/Anttila_et_al_Khuvsgul_2024/Supplementary_Information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F56D6D3-9EAB-2645-953D-8C144D03C0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4290D512-2AF7-8A4F-846C-55F3A56B9C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="720" windowWidth="27640" windowHeight="16180" xr2:uid="{E023F984-08FA-3B4B-9571-328833929427}"/>
+    <workbookView xWindow="27960" yWindow="-22180" windowWidth="27640" windowHeight="16180" xr2:uid="{E023F984-08FA-3B4B-9571-328833929427}"/>
   </bookViews>
   <sheets>
     <sheet name="Khuvsgul inputs" sheetId="1" r:id="rId1"/>
     <sheet name="Lithology parameters" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -602,7 +602,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B15"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -715,7 +715,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -741,7 +741,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -767,7 +767,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -787,7 +787,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -859,7 +859,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>